<commit_message>
[IMP] rework on supplier list report header
</commit_message>
<xml_diff>
--- a/pabi_procurement_report/xlsx_template/xlsx_report_pabi_supplier_list.xlsx
+++ b/pabi_procurement_report/xlsx_template/xlsx_report_pabi_supplier_list.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neunghathai\Desktop\Report Pabi\รายการแก้ไข\New folder (2)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siraph/Documents/pabi/pb2_addons/pabi_procurement_report/xlsx_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>ลำดับ</t>
   </si>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -471,52 +471,50 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.36328125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" style="4" customWidth="1"/>
     <col min="2" max="7" width="20" style="5" customWidth="1"/>
     <col min="8" max="8" width="25" style="5" customWidth="1"/>
     <col min="9" max="9" width="20" style="5" customWidth="1"/>
-    <col min="10" max="10" width="11.54296875" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="8.81640625" style="1"/>
+    <col min="10" max="10" width="11.5" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
     </row>
-    <row r="2" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>3</v>
-      </c>
+    <row r="5" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="9"/>
       <c r="B5" s="6"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" s="9"/>
       <c r="B6" s="6"/>
     </row>
-    <row r="7" spans="1:10" s="8" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="8" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -548,7 +546,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -559,7 +557,7 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -570,7 +568,7 @@
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -581,7 +579,7 @@
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11" s="3"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -592,7 +590,7 @@
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12" s="3"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>

</xml_diff>